<commit_message>
Updated Combined Project Proposal
</commit_message>
<xml_diff>
--- a/documentation/CENG355/ProposalContentRadio.xlsx
+++ b/documentation/CENG355/ProposalContentRadio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="170" windowWidth="14810" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="DataEntry" sheetId="1" r:id="rId1"/>
     <sheet name="DataBase" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -74,41 +74,132 @@
     <t>Speaker Bonnet &amp; FM Tuner Evaluation Board - Si4703</t>
   </si>
   <si>
-    <t>FM Radio Application</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Bluetooth in wireless communication. (n.d.). Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/1007414/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lumpkins, W. (n.d.). The MobiAria Wireless Bluetooth Speaker. Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/6685931/               </t>
-  </si>
-  <si>
-    <t>To make speakers amplified and output the raido signals from the FM Radio</t>
-  </si>
-  <si>
     <t>FM Tuner Evaluation Board (Aldo Ndreu), Speaker Bonnet (Ryan Antolin)</t>
   </si>
   <si>
-    <t>Firebase: Radio Stations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPARKFUN FM TUNER EVALUATION BOARD - SI4703 (https://elmwoodelectronics.ca/products/12938) Used for obtaining the radio stations. Adafruit I2S 3W Stereo Speaker Bonnet for Raspberry Pi - Mini Kit (https://www.adafruit.com/product/3346) Used for amplyifing audio from the PI. </t>
-  </si>
-  <si>
-    <t>This project is to connect from a mobile connection that can play audio towards the speaker bonnet. This is so that it can play audio in a speaker from the bonnent. It will amplify the audio so it can play in areas that you usually cannot hear with your mobile speakers.</t>
-  </si>
-  <si>
-    <t>This project is to be able to connect to a speaker via FM Radio. How this works is that you take a mobile device and connect to the database in order for the FM Radio to play through the speaker bonnet.</t>
+    <t>Our end solution and goal for this project is to use an amplified speaker and output the radio signal stations from the FM Radio sensor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lumpkins, W. (n.d.). The MobiAria Wireless Bluetooth Speaker. Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/6685931/
+Bodson, D. (n.d.). Digital Audio Around the World. Retrieved from http://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=5641649
+Pauli, M. (2017, May 5). Miniaturized Millimeter-Wave Radar Sensor for High-Accuracy Applications. Retrieved from http://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=7885501               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bluetooth in wireless communication. (n.d.). Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/1007414/
+SparkFun FM Tuner Evaluation Board - Si4703. (n.d.). Retrieved from https://www.sparkfun.com/products/12938
+</t>
+  </si>
+  <si>
+    <t>One of the products being used will be the FM evaluation board tuner chip. This device does more then tuning into FM stations, it can also detect both data service and radio broadcast data service. It can also be used to display station id and song to the user as well as have great filtering and carrying detection. This board will be able to pick up multiple radio stations and makes a great tool in order for it to be implemented with a Raspberry Pi. By using a speaker bonnet that acts as the output for this sensor, that is the primary source in which the sound will be coming from. It will amplify the audio so it can play in areas that you usually cannot hear with your mobile speakers.</t>
+  </si>
+  <si>
+    <t>This project which we will be creating will be able to connect to a speaker via FM Radio. How this  will work is by taking a mobile device and connecting to the database in order for the FM Radio stations to play through the speaker bonnet.</t>
+  </si>
+  <si>
+    <t>SparkFun Electronics (For Parts), Elmwood Electronics (For Parts), Prototype Lab (For Extra Help)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting or selecting different FM radio stations, Favorite different FM radio stations, Displays song or station currently playing </t>
+  </si>
+  <si>
+    <t>FM radio stations, and possibly favorited stations. 
+Database Used: Firebase</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CanaKit Raspberry Pi 3 Complete Starter Kit - 32 GB Edition -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The platform in which we will be doing this project on.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SPARKFUN FM TUNER EVALUATION BOARD - SI4703 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Enables users to tune into FM radio stations.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">JUMPER WIRES - CONNECTED 6" (M/F, 20 PACK) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Used for connection between breadboard where sensor is attached to Raspberry Pi 3.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Adafruit I2S 3W Stereo Speaker Bonnet for Raspberry Pi - Mini Kit - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Speaker used for amplyifing audio from the Raspberry Pi 3. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +211,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,7 +320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,9 +353,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -289,6 +405,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,18 +600,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.85546875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="19.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="69.81640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -486,7 +619,7 @@
         <v>43136</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -494,7 +627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -502,7 +635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -510,7 +643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -518,84 +651,84 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -616,12 +749,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="116" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="str">
         <f>DataEntry!A1</f>
         <v>Submission Date</v>
@@ -683,7 +816,7 @@
         <v>Solution description</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <f>DataEntry!B1</f>
         <v>43136</v>
@@ -706,15 +839,16 @@
       </c>
       <c r="F2" s="2" t="str">
         <f>DataEntry!B6</f>
-        <v>Firebase: Radio Stations</v>
+        <v>FM radio stations, and possibly favorited stations. 
+Database Used: Firebase</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>DataEntry!B7</f>
-        <v>FM Radio Application</v>
+        <v xml:space="preserve">Setting or selecting different FM radio stations, Favorite different FM radio stations, Displays song or station currently playing </v>
       </c>
       <c r="H2" s="2" t="str">
         <f>DataEntry!B8</f>
-        <v>N/A</v>
+        <v>SparkFun Electronics (For Parts), Elmwood Electronics (For Parts), Prototype Lab (For Extra Help)</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>DataEntry!B9</f>
@@ -722,27 +856,34 @@
       </c>
       <c r="J2" s="2" t="str">
         <f>DataEntry!B10</f>
-        <v>This project is to be able to connect to a speaker via FM Radio. How this works is that you take a mobile device and connect to the database in order for the FM Radio to play through the speaker bonnet.</v>
+        <v>This project which we will be creating will be able to connect to a speaker via FM Radio. How this  will work is by taking a mobile device and connecting to the database in order for the FM Radio stations to play through the speaker bonnet.</v>
       </c>
       <c r="K2" s="2" t="str">
         <f>DataEntry!B11</f>
-        <v>This project is to connect from a mobile connection that can play audio towards the speaker bonnet. This is so that it can play audio in a speaker from the bonnent. It will amplify the audio so it can play in areas that you usually cannot hear with your mobile speakers.</v>
+        <v>One of the products being used will be the FM evaluation board tuner chip. This device does more then tuning into FM stations, it can also detect both data service and radio broadcast data service. It can also be used to display station id and song to the user as well as have great filtering and carrying detection. This board will be able to pick up multiple radio stations and makes a great tool in order for it to be implemented with a Raspberry Pi. By using a speaker bonnet that acts as the output for this sensor, that is the primary source in which the sound will be coming from. It will amplify the audio so it can play in areas that you usually cannot hear with your mobile speakers.</v>
       </c>
       <c r="L2" s="2" t="str">
         <f>DataEntry!B12</f>
-        <v>Bluetooth in wireless communication. (n.d.). Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/1007414/</v>
+        <v xml:space="preserve">Bluetooth in wireless communication. (n.d.). Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/1007414/
+SparkFun FM Tuner Evaluation Board - Si4703. (n.d.). Retrieved from https://www.sparkfun.com/products/12938
+</v>
       </c>
       <c r="M2" s="2" t="str">
         <f>DataEntry!B13</f>
-        <v xml:space="preserve">Lumpkins, W. (n.d.). The MobiAria Wireless Bluetooth Speaker. Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/6685931/               </v>
+        <v xml:space="preserve">Lumpkins, W. (n.d.). The MobiAria Wireless Bluetooth Speaker. Retrieved September 18, 2017, from http://ieeexplore.ieee.org/document/6685931/
+Bodson, D. (n.d.). Digital Audio Around the World. Retrieved from http://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=5641649
+Pauli, M. (2017, May 5). Miniaturized Millimeter-Wave Radar Sensor for High-Accuracy Applications. Retrieved from http://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=7885501               </v>
       </c>
       <c r="N2" s="2" t="str">
         <f>DataEntry!B14</f>
-        <v xml:space="preserve">SPARKFUN FM TUNER EVALUATION BOARD - SI4703 (https://elmwoodelectronics.ca/products/12938) Used for obtaining the radio stations. Adafruit I2S 3W Stereo Speaker Bonnet for Raspberry Pi - Mini Kit (https://www.adafruit.com/product/3346) Used for amplyifing audio from the PI. </v>
+        <v xml:space="preserve">CanaKit Raspberry Pi 3 Complete Starter Kit - 32 GB Edition - The platform in which we will be doing this project on.
+SPARKFUN FM TUNER EVALUATION BOARD - SI4703 - Enables users to tune into FM radio stations.
+JUMPER WIRES - CONNECTED 6" (M/F, 20 PACK) - Used for connection between breadboard where sensor is attached to Raspberry Pi 3.
+Adafruit I2S 3W Stereo Speaker Bonnet for Raspberry Pi - Mini Kit - Speaker used for amplyifing audio from the Raspberry Pi 3. </v>
       </c>
       <c r="O2" s="2" t="str">
         <f>DataEntry!B15</f>
-        <v>To make speakers amplified and output the raido signals from the FM Radio</v>
+        <v>Our end solution and goal for this project is to use an amplified speaker and output the radio signal stations from the FM Radio sensor.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>